<commit_message>
changed unit num of PPO
</commit_message>
<xml_diff>
--- a/rl_data/学習記録.xlsx
+++ b/rl_data/学習記録.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">学習記録</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">備考</t>
   </si>
   <si>
+    <t xml:space="preserve">追記</t>
+  </si>
+  <si>
     <t xml:space="preserve">12/18:12/19</t>
   </si>
   <si>
@@ -94,6 +97,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ドアヒンジの</t>
     </r>
@@ -111,17 +115,126 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">の設定が大きすぎた</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">UniPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">同上</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mlp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">の</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">を増やしてみた</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">層，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2048→64</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">数増やしすぎても逆効果かも </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PPO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">だと報酬の変化方向に動くはずなのでスパースだと無理な気がしてきた</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ゴミなので特にデータ出力せず</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -199,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,6 +322,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,18 +346,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,34 +377,60 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
add levorg nice learning data
</commit_message>
<xml_diff>
--- a/rl_data/学習記録.xlsx
+++ b/rl_data/学習記録.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">学習記録</t>
   </si>
@@ -121,6 +121,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">12/19/</t>
+  </si>
+  <si>
     <t xml:space="preserve">UniPC</t>
   </si>
   <si>
@@ -141,6 +144,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">の</t>
     </r>
@@ -158,6 +162,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">を増やしてみた</t>
     </r>
@@ -175,6 +180,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">層，</t>
     </r>
@@ -203,6 +209,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数増やしすぎても逆効果かも </t>
     </r>
@@ -220,12 +227,155 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">だと報酬の変化方向に動くはずなのでスパースだと無理な気がしてきた</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">ゴミなので特にデータ出力せず</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PPO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ヒンジ報酬，ドアノブ報酬のみ</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">報酬のスケールを小さくした</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ハンドルの付け根を引っ張って開けている様子</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">なんか惜しいので，ドアヒンジ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">friction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">と</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">dampng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">上げる，ドアノブ報酬上げる，ドアノブ付け根</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">urdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">修正
+ロボット自体の</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">damping</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">と速度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">limit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">考えたほうが良いかもしれない
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1000epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">くらいでこの動きが生まれ始めた様子</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">重み保存済み</t>
   </si>
 </sst>
 </file>
@@ -312,21 +462,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -346,91 +508,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="94.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="15.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>45279</v>
-      </c>
-      <c r="B3" s="0" t="s">
+    <row r="3" customFormat="false" ht="15.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>16</v>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>45280</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
1220 done, but wasnt better
</commit_message>
<xml_diff>
--- a/rl_data/学習記録.xlsx
+++ b/rl_data/学習記録.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">学習記録</t>
   </si>
@@ -250,6 +250,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ヒンジ報酬，ドアノブ報酬のみ</t>
     </r>
@@ -266,6 +267,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">なんか惜しいので，ドアヒンジ</t>
     </r>
@@ -283,6 +285,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">と</t>
     </r>
@@ -300,6 +303,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">上げる，ドアノブ報酬上げる，ドアノブ付け根</t>
     </r>
@@ -317,6 +321,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">修正
 ロボット自体の</t>
@@ -335,6 +340,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">と速度</t>
     </r>
@@ -352,6 +358,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">考えたほうが良いかもしれない
 </t>
@@ -370,12 +377,32 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">くらいでこの動きが生まれ始めた様子</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">重み保存済み</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">dof</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">も初期位置ランダム要素を加えてみたらどうなるだろうか？</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -462,7 +489,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -483,11 +510,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,10 +531,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -601,17 +624,22 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>